<commit_message>
update gdscript config table tool
</commit_message>
<xml_diff>
--- a/config_table/excels/people.xlsx
+++ b/config_table/excels/people.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
-    <sheet name="people" sheetId="2" r:id="rId5"/>
+    <sheet name="people" sheetId="9" r:id="rId5"/>
+    <sheet name="sub" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="26">
   <si>
     <t xml:space="preserve">姓名</t>
   </si>
@@ -47,47 +48,63 @@
   </si>
   <si>
     <t xml:space="preserve">张三</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">李四</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">王五</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">陈六</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">赵七</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">陈府井3号</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">六大胡同4号</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">浅水滩1号</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">太阳弯403号</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">第一高级中学教师生活区103号</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">138456456456</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">注释</t>
+  </si>
+  <si>
+    <t xml:space="preserve">explained1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">工作</t>
+  </si>
+  <si>
+    <t xml:space="preserve">job</t>
   </si>
 </sst>
 </file>
@@ -95,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -106,21 +123,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -145,6 +147,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="000000"/>
       <name val="Calibri"/>
     </font>
@@ -163,13 +185,58 @@
       <color rgb="FFFFFF"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -307,38 +374,68 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -653,7 +750,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -664,121 +761,180 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5625" style="7" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5625" style="7" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5625" style="7" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.5625" style="7" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.5625" style="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="24" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" ht="14" customHeight="1">
+      <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5625" style="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5625" style="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5625" style="17" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5625" style="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5625" style="17" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="24" customHeight="1">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="14" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="20" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1">
         <v>17</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
         <v>16</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update config table plugin
</commit_message>
<xml_diff>
--- a/config_table/excels/people.xlsx
+++ b/config_table/excels/people.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
-    <sheet name="people" sheetId="25" r:id="rId6"/>
-    <sheet name="sub" sheetId="26" r:id="rId7"/>
+    <sheet name="people" sheetId="27" r:id="rId8"/>
+    <sheet name="sub" sheetId="28" r:id="rId9"/>
+    <sheet name="sub_sub" sheetId="29" r:id="rId10"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -234,8 +235,48 @@
 </comments>
 </file>
 
+<file path=xl/comments27.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <t xml:space="preserve">某人的姓名</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <t xml:space="preserve">注释而已</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <t xml:space="preserve">真实的地址</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments28.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <t xml:space="preserve">用于写下工作的信息</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="27">
   <si>
     <t xml:space="preserve">姓名</t>
   </si>
@@ -325,6 +366,9 @@
   </si>
   <si>
     <t xml:space="preserve">job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
   </si>
 </sst>
 </file>
@@ -332,7 +376,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="57" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -383,6 +427,26 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -754,7 +818,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -912,6 +976,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -944,6 +1020,14 @@
 </file>
 
 <file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
 </file>
 
@@ -1274,7 +1358,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1285,61 +1369,61 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5625" style="49" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5625" style="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5625" style="49" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.5625" style="49" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.5625" style="49" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.5625" style="53" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5625" style="53" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5625" style="53" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5625" style="53" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5625" style="53" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="24" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="54" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="55" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="14" customHeight="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="56" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1435,7 +1519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1446,21 +1530,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5625" style="49" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.5625" style="53" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="24" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="54" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="55" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" ht="14" customHeight="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1469,4 +1553,38 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5625" style="53" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="24" customHeight="1">
+      <c r="A1" s="54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" ht="14" customHeight="1">
+      <c r="A3" s="56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update config table tool.
</commit_message>
<xml_diff>
--- a/config_table/excels/people.xlsx
+++ b/config_table/excels/people.xlsx
@@ -1,21 +1,164 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView tabRatio="600"/>
+  </bookViews>
   <sheets>
-    <sheet name="people" sheetId="1" r:id="rId1"/>
-    <sheet name="sub" sheetId="2" r:id="rId2"/>
-    <sheet name="sub_sub" sheetId="3" r:id="rId3"/>
+    <sheet name="people" sheetId="4" r:id="rId7"/>
+    <sheet name="sub" sheetId="5" r:id="rId8"/>
+    <sheet name="sub_sub" sheetId="6" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <t xml:space="preserve">某人的姓名</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <t xml:space="preserve">注释而已</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <t xml:space="preserve">真实的地址</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <t xml:space="preserve">用于写下工作的信息</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
+  <si>
+    <t xml:space="preserve">姓名</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">注释</t>
+  </si>
+  <si>
+    <t xml:space="preserve">explained1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">年龄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">家庭住址</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">手机号</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">张三</t>
+  </si>
+  <si>
+    <t xml:space="preserve">李四</t>
+  </si>
+  <si>
+    <t xml:space="preserve">王五</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陈六</t>
+  </si>
+  <si>
+    <t xml:space="preserve">赵七</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res://config_table/ConfigHelper.gd
+asdsad
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陈府井3号</t>
+  </si>
+  <si>
+    <t xml:space="preserve">第一高级中学教师生活区103号</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浅水滩1号</t>
+  </si>
+  <si>
+    <t xml:space="preserve">六大胡同4号</t>
+  </si>
+  <si>
+    <t xml:space="preserve">太阳弯403号</t>
+  </si>
+  <si>
+    <t xml:space="preserve">138456456456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">工作</t>
+  </si>
+  <si>
+    <t xml:space="preserve">job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -23,16 +166,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00E7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00A9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00525252"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00525252"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -40,12 +233,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -53,6 +334,14 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -274,7 +563,7 @@
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
-          <a:sp3d>
+          <a:sp3d prstMaterial="warmMatte">
             <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
@@ -334,7 +623,7 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr/>
-      <a:bodyPr/>
+      <a:bodyPr rtlCol="0"/>
       <a:lstStyle/>
       <a:style>
         <a:lnRef idx="1">
@@ -353,7 +642,7 @@
     </a:spDef>
     <a:lnDef>
       <a:spPr/>
-      <a:bodyPr/>
+      <a:bodyPr rtlCol="0"/>
       <a:lstStyle/>
       <a:style>
         <a:lnRef idx="2">
@@ -375,217 +664,238 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5625" style="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>姓名</v>
-      </c>
-      <c r="B1" t="str">
-        <v>注释</v>
-      </c>
-      <c r="C1" t="str">
-        <v>年龄</v>
-      </c>
-      <c r="D1" t="str">
-        <v>家庭住址</v>
-      </c>
-      <c r="E1" t="str">
-        <v>手机号</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>name</v>
-      </c>
-      <c r="B2" t="str">
-        <v>explained1</v>
-      </c>
-      <c r="C2" t="str">
-        <v>age</v>
-      </c>
-      <c r="D2" t="str">
-        <v>address</v>
-      </c>
-      <c r="E2" t="str">
-        <v>phone</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>String</v>
-      </c>
-      <c r="B3" t="str">
-        <v>String</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Real</v>
-      </c>
-      <c r="D3" t="str">
-        <v>String</v>
-      </c>
-      <c r="E3" t="str">
-        <v>String</v>
+    <row r="1" ht="24" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="14" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
-        <v>张三</v>
-      </c>
-      <c r="B4" t="str">
-        <v>asdasd</v>
-      </c>
-      <c r="C4" t="str">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="str">
-        <v>陈府井3号</v>
-      </c>
-      <c r="E4" t="str">
-        <v>138456456456</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>李四</v>
-      </c>
-      <c r="B5" t="str">
-        <v>asdasd</v>
-      </c>
-      <c r="C5" t="str">
-        <v>15</v>
-      </c>
-      <c r="D5" t="str">
-        <v>第一高级中学教师生活区103号</v>
-      </c>
-      <c r="E5" t="str">
-        <v>138456456456</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>王五</v>
-      </c>
-      <c r="B6" t="str">
-        <v>asdasd</v>
-      </c>
-      <c r="C6" t="str">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="str">
-        <v>浅水滩1号</v>
-      </c>
-      <c r="E6" t="str">
-        <v>138456456456</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>陈六</v>
-      </c>
-      <c r="B7" t="str">
-        <v>asdasd</v>
-      </c>
-      <c r="C7" t="str">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="str">
-        <v>六大胡同4号</v>
-      </c>
-      <c r="E7" t="str">
-        <v>138456456456</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>赵七</v>
-      </c>
-      <c r="B8" t="str">
-        <v>asdasd</v>
-      </c>
-      <c r="C8" t="str">
-        <v>16</v>
-      </c>
-      <c r="D8" t="str">
-        <v>太阳弯403号</v>
-      </c>
-      <c r="E8" t="str">
-        <v>138456456456</v>
-      </c>
-    </row>
-    <row r="9" xml:space="preserve">
-      <c r="A9" t="str" xml:space="preserve">
-        <v xml:space="preserve">res://config_table/ConfigHelper.gd
-asdsad
-</v>
-      </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5625" style="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>工作</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>job</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>String</v>
+    <row r="1" ht="24" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" ht="14" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5625" style="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>test</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>test</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>String</v>
+    <row r="1" ht="24" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" ht="14" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>